<commit_message>
update pie chart to report
</commit_message>
<xml_diff>
--- a/templates/employee_export_template.xlsx
+++ b/templates/employee_export_template.xlsx
@@ -33,33 +33,20 @@
     <t>Tên dự án</t>
   </si>
   <si>
-    <r>
-      <t>Thời gian tham gia</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (ngày)</t>
-    </r>
-  </si>
-  <si>
     <t>Tên nhân viên: ABC</t>
   </si>
   <si>
     <t>BÁO CÁO DỰ ÁN THAM GIA CỦA NHÂN VIÊN</t>
+  </si>
+  <si>
+    <t>Số giờ thực hiện</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,14 +73,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -436,7 +415,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,7 +427,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -458,7 +437,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -469,7 +448,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>